<commit_message>
six new hats, sentan ty message
</commit_message>
<xml_diff>
--- a/CustomHatsGM.xlsx
+++ b/CustomHatsGM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherHats-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F933BF91-A977-4553-8EDC-CFFB1267E502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B7D82F-7406-4634-BAB5-E7EF96D1A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="6255" windowWidth="23730" windowHeight="8730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="2520" windowWidth="24345" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hats" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="354">
   <si>
     <t>resource</t>
   </si>
@@ -355,9 +355,6 @@
     <t>ぴんちゃん</t>
   </si>
   <si>
-    <t>先端恐怖症</t>
-  </si>
-  <si>
     <t>瀬戸あさひ</t>
   </si>
   <si>
@@ -1034,6 +1031,63 @@
   </si>
   <si>
     <t>天羽よつは</t>
+  </si>
+  <si>
+    <t>akameta.png</t>
+  </si>
+  <si>
+    <t>akameta_climb.png</t>
+  </si>
+  <si>
+    <t>nekodukimio.png</t>
+  </si>
+  <si>
+    <t>nekodukimio_back.png</t>
+  </si>
+  <si>
+    <t>nekodukimio_climb.png</t>
+  </si>
+  <si>
+    <t>only.png</t>
+  </si>
+  <si>
+    <t>only_climb.png</t>
+  </si>
+  <si>
+    <t>ooharamen.png</t>
+  </si>
+  <si>
+    <t>ooharamen_climb.png</t>
+  </si>
+  <si>
+    <t>santos.png</t>
+  </si>
+  <si>
+    <t>santos_climb.png</t>
+  </si>
+  <si>
+    <t>sunazame.png</t>
+  </si>
+  <si>
+    <t>アカメタ</t>
+  </si>
+  <si>
+    <t>猫月みお</t>
+  </si>
+  <si>
+    <t>おんりー</t>
+  </si>
+  <si>
+    <t>おおはらMEN</t>
+  </si>
+  <si>
+    <t>サントス</t>
+  </si>
+  <si>
+    <t>スナザメ</t>
+  </si>
+  <si>
+    <t>先端恐怖症\n主催有難うございました！</t>
   </si>
 </sst>
 </file>
@@ -1351,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,7 +1452,7 @@
         <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1415,7 +1469,7 @@
         <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -1432,7 +1486,7 @@
         <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -1449,7 +1503,7 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1466,7 +1520,7 @@
         <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -1483,7 +1537,7 @@
         <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -1500,7 +1554,7 @@
         <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -1514,7 +1568,7 @@
         <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -1531,7 +1585,7 @@
         <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D10" t="s">
         <v>44</v>
@@ -1548,7 +1602,7 @@
         <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
@@ -1565,7 +1619,7 @@
         <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -1585,7 +1639,7 @@
         <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
@@ -1602,7 +1656,7 @@
         <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -1619,7 +1673,7 @@
         <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D15" t="s">
         <v>55</v>
@@ -1636,7 +1690,7 @@
         <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
@@ -1653,7 +1707,7 @@
         <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D17" t="s">
         <v>59</v>
@@ -1670,7 +1724,7 @@
         <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D18" t="s">
         <v>61</v>
@@ -1687,7 +1741,7 @@
         <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -1704,7 +1758,7 @@
         <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D20" t="s">
         <v>65</v>
@@ -1721,7 +1775,7 @@
         <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D21" t="s">
         <v>67</v>
@@ -1738,7 +1792,7 @@
         <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D22" t="s">
         <v>69</v>
@@ -1755,7 +1809,7 @@
         <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D23" t="s">
         <v>71</v>
@@ -1775,7 +1829,7 @@
         <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D24" t="s">
         <v>74</v>
@@ -1792,7 +1846,7 @@
         <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D25" t="s">
         <v>76</v>
@@ -1812,7 +1866,7 @@
         <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D26" t="s">
         <v>79</v>
@@ -1829,7 +1883,7 @@
         <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D27" t="s">
         <v>81</v>
@@ -1846,7 +1900,7 @@
         <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D28" t="s">
         <v>83</v>
@@ -1863,7 +1917,7 @@
         <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D29" t="s">
         <v>85</v>
@@ -1880,7 +1934,7 @@
         <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D30" t="s">
         <v>87</v>
@@ -1897,16 +1951,16 @@
         <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D31" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" t="s">
         <v>290</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>291</v>
-      </c>
-      <c r="F31" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,13 +1971,13 @@
         <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" t="s">
         <v>115</v>
-      </c>
-      <c r="F35" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,13 +1988,13 @@
         <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" t="s">
         <v>117</v>
-      </c>
-      <c r="F36" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1951,152 +2005,172 @@
         <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" t="s">
         <v>119</v>
       </c>
-      <c r="F37" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>285</v>
+      </c>
+      <c r="D38" t="s">
         <v>120</v>
+      </c>
+      <c r="F38" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
         <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F39" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
         <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F40" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
         <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
         <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
         <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
         <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="E45" t="s">
+        <v>135</v>
       </c>
       <c r="F45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>353</v>
       </c>
       <c r="B46" t="s">
         <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E46" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F46" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,16 +2181,16 @@
         <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D47" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E47" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F47" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,16 +2201,13 @@
         <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F48" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,13 +2218,13 @@
         <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2164,13 +2235,13 @@
         <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D50" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F50" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2181,33 +2252,36 @@
         <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="E51" t="s">
+        <v>150</v>
       </c>
       <c r="F51" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" t="s">
-        <v>286</v>
-      </c>
-      <c r="D52" t="s">
-        <v>150</v>
-      </c>
-      <c r="E52" t="s">
         <v>151</v>
       </c>
-      <c r="F52" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>285</v>
+      </c>
+      <c r="D55" t="s">
         <v>152</v>
+      </c>
+      <c r="E55" t="s">
+        <v>153</v>
+      </c>
+      <c r="F55" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,56 +2292,53 @@
         <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F56" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B57" t="s">
         <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D57" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E57" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F57" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>289</v>
+        <v>202</v>
       </c>
       <c r="B58" t="s">
         <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D58" t="s">
-        <v>158</v>
-      </c>
-      <c r="E58" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F58" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2278,13 +2349,13 @@
         <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F59" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2295,13 +2366,13 @@
         <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D60" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F60" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2312,13 +2383,16 @@
         <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="E61" t="s">
+        <v>167</v>
       </c>
       <c r="F61" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2329,16 +2403,16 @@
         <v>97</v>
       </c>
       <c r="C62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D62" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E62" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F62" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2349,16 +2423,13 @@
         <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D63" t="s">
-        <v>170</v>
-      </c>
-      <c r="E63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F63" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2369,13 +2440,13 @@
         <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D64" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F64" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2386,13 +2457,13 @@
         <v>97</v>
       </c>
       <c r="C65" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D65" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F65" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,13 +2474,13 @@
         <v>97</v>
       </c>
       <c r="C66" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D66" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F66" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2420,13 +2491,13 @@
         <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D67" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,13 +2508,13 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D68" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F68" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2454,13 +2525,16 @@
         <v>97</v>
       </c>
       <c r="C69" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D69" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+      <c r="E69" t="s">
+        <v>185</v>
       </c>
       <c r="F69" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2471,16 +2545,13 @@
         <v>97</v>
       </c>
       <c r="C70" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D70" t="s">
-        <v>185</v>
-      </c>
-      <c r="E70" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F70" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2491,13 +2562,13 @@
         <v>97</v>
       </c>
       <c r="C71" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D71" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F71" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,13 +2579,13 @@
         <v>97</v>
       </c>
       <c r="C72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D72" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F72" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,13 +2596,13 @@
         <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D73" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F73" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,13 +2613,13 @@
         <v>97</v>
       </c>
       <c r="C74" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D74" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F74" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2559,81 +2630,81 @@
         <v>97</v>
       </c>
       <c r="C75" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D75" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F75" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>220</v>
-      </c>
-      <c r="B76" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" t="s">
-        <v>286</v>
-      </c>
-      <c r="D76" t="s">
         <v>198</v>
       </c>
-      <c r="F76" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>292</v>
+      </c>
+      <c r="B79" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" t="s">
+        <v>285</v>
+      </c>
+      <c r="D79" t="s">
         <v>293</v>
       </c>
-      <c r="B80" t="s">
-        <v>97</v>
-      </c>
-      <c r="C80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="F79" t="s">
         <v>294</v>
       </c>
-      <c r="F80" t="s">
-        <v>295</v>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>296</v>
+      </c>
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>285</v>
+      </c>
+      <c r="D83" t="s">
+        <v>305</v>
+      </c>
+      <c r="F83" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B84" t="s">
         <v>97</v>
       </c>
       <c r="C84" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D84" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F84" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B85" t="s">
         <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D85" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F85" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2644,13 +2715,13 @@
         <v>97</v>
       </c>
       <c r="C86" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D86" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F86" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2661,13 +2732,13 @@
         <v>97</v>
       </c>
       <c r="C87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D87" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F87" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2678,13 +2749,13 @@
         <v>97</v>
       </c>
       <c r="C88" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D88" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F88" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2695,13 +2766,16 @@
         <v>97</v>
       </c>
       <c r="C89" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D89" t="s">
-        <v>316</v>
+        <v>317</v>
+      </c>
+      <c r="E89" t="s">
+        <v>318</v>
       </c>
       <c r="F89" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2712,16 +2786,16 @@
         <v>97</v>
       </c>
       <c r="C90" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D90" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E90" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F90" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2732,16 +2806,13 @@
         <v>97</v>
       </c>
       <c r="C91" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D91" t="s">
-        <v>321</v>
-      </c>
-      <c r="E91" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F91" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2752,33 +2823,36 @@
         <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D92" t="s">
-        <v>324</v>
+        <v>325</v>
+      </c>
+      <c r="E92" t="s">
+        <v>326</v>
       </c>
       <c r="F92" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="B93" t="s">
         <v>97</v>
       </c>
       <c r="C93" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D93" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E93" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F93" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2789,33 +2863,115 @@
         <v>97</v>
       </c>
       <c r="C94" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D94" t="s">
-        <v>329</v>
-      </c>
-      <c r="E94" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F94" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>347</v>
+      </c>
+      <c r="B98" t="s">
+        <v>97</v>
+      </c>
+      <c r="C98" t="s">
+        <v>285</v>
+      </c>
+      <c r="D98" t="s">
         <v>335</v>
       </c>
-      <c r="B95" t="s">
-        <v>97</v>
-      </c>
-      <c r="C95" t="s">
-        <v>286</v>
-      </c>
-      <c r="D95" t="s">
-        <v>332</v>
-      </c>
-      <c r="F95" t="s">
-        <v>333</v>
+      <c r="F98" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>348</v>
+      </c>
+      <c r="B99" t="s">
+        <v>97</v>
+      </c>
+      <c r="C99" t="s">
+        <v>285</v>
+      </c>
+      <c r="D99" t="s">
+        <v>337</v>
+      </c>
+      <c r="E99" t="s">
+        <v>338</v>
+      </c>
+      <c r="F99" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>349</v>
+      </c>
+      <c r="B100" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" t="s">
+        <v>285</v>
+      </c>
+      <c r="D100" t="s">
+        <v>340</v>
+      </c>
+      <c r="F100" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>350</v>
+      </c>
+      <c r="B101" t="s">
+        <v>97</v>
+      </c>
+      <c r="C101" t="s">
+        <v>285</v>
+      </c>
+      <c r="D101" t="s">
+        <v>342</v>
+      </c>
+      <c r="F101" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>351</v>
+      </c>
+      <c r="B102" t="s">
+        <v>97</v>
+      </c>
+      <c r="C102" t="s">
+        <v>285</v>
+      </c>
+      <c r="D102" t="s">
+        <v>344</v>
+      </c>
+      <c r="F102" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>352</v>
+      </c>
+      <c r="B103" t="s">
+        <v>97</v>
+      </c>
+      <c r="C103" t="s">
+        <v>285</v>
+      </c>
+      <c r="D103" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2867,357 +3023,357 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" t="s">
         <v>229</v>
-      </c>
-      <c r="G6" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E18" t="s">
+        <v>256</v>
+      </c>
+      <c r="F18" t="s">
         <v>257</v>
-      </c>
-      <c r="F18" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" t="s">
         <v>284</v>
       </c>
-      <c r="B21" t="s">
-        <v>287</v>
-      </c>
-      <c r="C21" t="s">
-        <v>285</v>
-      </c>
       <c r="D21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sentan thank you message
</commit_message>
<xml_diff>
--- a/CustomHatsGM.xlsx
+++ b/CustomHatsGM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherHats-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B7D82F-7406-4634-BAB5-E7EF96D1A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0ABDB6-AFF0-414C-B98A-152A0B3337A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="2520" windowWidth="24345" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="7035" windowWidth="20475" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hats" sheetId="1" r:id="rId1"/>
@@ -355,6 +355,9 @@
     <t>ぴんちゃん</t>
   </si>
   <si>
+    <t>先端恐怖症</t>
+  </si>
+  <si>
     <t>瀬戸あさひ</t>
   </si>
   <si>
@@ -1085,9 +1088,6 @@
   </si>
   <si>
     <t>スナザメ</t>
-  </si>
-  <si>
-    <t>先端恐怖症\n主催有難うございました！</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1452,7 @@
         <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1469,7 +1469,7 @@
         <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -1486,7 +1486,7 @@
         <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -1503,7 +1503,7 @@
         <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1520,7 +1520,7 @@
         <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -1537,7 +1537,7 @@
         <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -1554,7 +1554,7 @@
         <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -1568,7 +1568,7 @@
         <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -1585,7 +1585,7 @@
         <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D10" t="s">
         <v>44</v>
@@ -1602,7 +1602,7 @@
         <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
@@ -1619,7 +1619,7 @@
         <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -1639,7 +1639,7 @@
         <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
@@ -1656,7 +1656,7 @@
         <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -1673,7 +1673,7 @@
         <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D15" t="s">
         <v>55</v>
@@ -1690,7 +1690,7 @@
         <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
@@ -1707,7 +1707,7 @@
         <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D17" t="s">
         <v>59</v>
@@ -1724,7 +1724,7 @@
         <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D18" t="s">
         <v>61</v>
@@ -1741,7 +1741,7 @@
         <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -1758,7 +1758,7 @@
         <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D20" t="s">
         <v>65</v>
@@ -1775,7 +1775,7 @@
         <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D21" t="s">
         <v>67</v>
@@ -1792,7 +1792,7 @@
         <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D22" t="s">
         <v>69</v>
@@ -1809,7 +1809,7 @@
         <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D23" t="s">
         <v>71</v>
@@ -1829,7 +1829,7 @@
         <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D24" t="s">
         <v>74</v>
@@ -1846,7 +1846,7 @@
         <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D25" t="s">
         <v>76</v>
@@ -1866,7 +1866,7 @@
         <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D26" t="s">
         <v>79</v>
@@ -1883,7 +1883,7 @@
         <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D27" t="s">
         <v>81</v>
@@ -1900,7 +1900,7 @@
         <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D28" t="s">
         <v>83</v>
@@ -1917,7 +1917,7 @@
         <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D29" t="s">
         <v>85</v>
@@ -1934,7 +1934,7 @@
         <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D30" t="s">
         <v>87</v>
@@ -1951,16 +1951,16 @@
         <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D31" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E31" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F31" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,13 +1971,13 @@
         <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1988,13 +1988,13 @@
         <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,13 +2005,13 @@
         <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2022,13 +2022,13 @@
         <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,13 +2039,13 @@
         <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,13 +2056,13 @@
         <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2073,13 +2073,13 @@
         <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,13 +2090,13 @@
         <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F42" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,13 +2107,13 @@
         <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,13 +2124,13 @@
         <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,837 +2141,837 @@
         <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D45" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E45" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>353</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
         <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E47" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F47" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
         <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F48" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
         <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D50" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F50" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
         <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F51" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>201</v>
+      </c>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>286</v>
+      </c>
+      <c r="D55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" t="s">
+        <v>154</v>
+      </c>
+      <c r="F55" t="s">
         <v>200</v>
-      </c>
-      <c r="B55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" t="s">
-        <v>285</v>
-      </c>
-      <c r="D55" t="s">
-        <v>152</v>
-      </c>
-      <c r="E55" t="s">
-        <v>153</v>
-      </c>
-      <c r="F55" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B56" t="s">
         <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D56" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E56" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F56" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B57" t="s">
         <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F57" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B58" t="s">
         <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F58" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B59" t="s">
         <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F59" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B60" t="s">
         <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F60" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
         <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D61" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E61" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F61" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B62" t="s">
         <v>97</v>
       </c>
       <c r="C62" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D62" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E62" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F62" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B63" t="s">
         <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D63" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F63" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B64" t="s">
         <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D64" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F64" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B65" t="s">
         <v>97</v>
       </c>
       <c r="C65" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D65" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F65" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B66" t="s">
         <v>97</v>
       </c>
       <c r="C66" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D66" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F66" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B67" t="s">
         <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F67" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B68" t="s">
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D68" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F68" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B69" t="s">
         <v>97</v>
       </c>
       <c r="C69" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D69" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F69" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B70" t="s">
         <v>97</v>
       </c>
       <c r="C70" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D70" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F70" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B71" t="s">
         <v>97</v>
       </c>
       <c r="C71" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D71" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F71" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B72" t="s">
         <v>97</v>
       </c>
       <c r="C72" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D72" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F72" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D73" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F73" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B74" t="s">
         <v>97</v>
       </c>
       <c r="C74" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D74" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F74" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B75" t="s">
         <v>97</v>
       </c>
       <c r="C75" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D75" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F75" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B79" t="s">
         <v>97</v>
       </c>
       <c r="C79" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D79" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F79" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B83" t="s">
         <v>97</v>
       </c>
       <c r="C83" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D83" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F83" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B84" t="s">
         <v>97</v>
       </c>
       <c r="C84" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D84" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F84" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B85" t="s">
         <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D85" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F85" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B86" t="s">
         <v>97</v>
       </c>
       <c r="C86" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D86" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F86" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B87" t="s">
         <v>97</v>
       </c>
       <c r="C87" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D87" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F87" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B88" t="s">
         <v>97</v>
       </c>
       <c r="C88" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D88" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F88" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B89" t="s">
         <v>97</v>
       </c>
       <c r="C89" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D89" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E89" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F89" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B90" t="s">
         <v>97</v>
       </c>
       <c r="C90" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D90" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E90" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F90" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B91" t="s">
         <v>97</v>
       </c>
       <c r="C91" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D91" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F91" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B92" t="s">
         <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D92" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E92" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F92" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B93" t="s">
         <v>97</v>
       </c>
       <c r="C93" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D93" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E93" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F93" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B94" t="s">
         <v>97</v>
       </c>
       <c r="C94" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D94" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F94" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B98" t="s">
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D98" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F98" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B99" t="s">
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D99" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E99" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F99" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B100" t="s">
         <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D100" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F100" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B101" t="s">
         <v>97</v>
       </c>
       <c r="C101" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D101" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B102" t="s">
         <v>97</v>
       </c>
       <c r="C102" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D102" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F102" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B103" t="s">
         <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D103" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -3023,357 +3023,357 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" t="s">
         <v>221</v>
-      </c>
-      <c r="F2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" t="s">
         <v>223</v>
-      </c>
-      <c r="F3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F4" t="s">
         <v>225</v>
-      </c>
-      <c r="F4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" t="s">
         <v>227</v>
-      </c>
-      <c r="F5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" t="s">
         <v>230</v>
-      </c>
-      <c r="F6" t="s">
-        <v>228</v>
-      </c>
-      <c r="G6" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F7" t="s">
         <v>232</v>
-      </c>
-      <c r="F7" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" t="s">
         <v>235</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>234</v>
-      </c>
-      <c r="G8" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" t="s">
         <v>237</v>
-      </c>
-      <c r="F9" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F10" t="s">
         <v>239</v>
-      </c>
-      <c r="F10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" t="s">
         <v>287</v>
       </c>
-      <c r="B11" t="s">
-        <v>286</v>
-      </c>
       <c r="C11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" t="s">
         <v>241</v>
-      </c>
-      <c r="F11" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C12" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" t="s">
         <v>243</v>
-      </c>
-      <c r="F12" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D13" t="s">
+        <v>246</v>
+      </c>
+      <c r="F13" t="s">
         <v>245</v>
-      </c>
-      <c r="F13" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C14" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D14" t="s">
+        <v>248</v>
+      </c>
+      <c r="F14" t="s">
         <v>247</v>
-      </c>
-      <c r="F14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B15" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C15" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D15" t="s">
+        <v>251</v>
+      </c>
+      <c r="F15" t="s">
         <v>250</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>249</v>
-      </c>
-      <c r="G15" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D16" t="s">
+        <v>254</v>
+      </c>
+      <c r="F16" t="s">
         <v>253</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>252</v>
-      </c>
-      <c r="G16" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D17" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" t="s">
         <v>255</v>
-      </c>
-      <c r="F17" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C18" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E18" t="s">
+        <v>257</v>
+      </c>
+      <c r="F18" t="s">
         <v>258</v>
-      </c>
-      <c r="E18" t="s">
-        <v>256</v>
-      </c>
-      <c r="F18" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B19" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C19" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D19" t="s">
+        <v>261</v>
+      </c>
+      <c r="F19" t="s">
         <v>260</v>
-      </c>
-      <c r="F19" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B20" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F20" t="s">
         <v>262</v>
-      </c>
-      <c r="F20" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C21" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D21" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" t="s">
         <v>264</v>
-      </c>
-      <c r="F21" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>